<commit_message>
Add unit price in for accounting range of date and add date in item list filter export
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -32,7 +32,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2020-07-09</t>
+    <t>2020-07-13</t>
   </si>
   <si>
     <t>Main Category</t>
@@ -2783,6 +2783,12 @@
     <t>CON-CON_1328</t>
   </si>
   <si>
+    <t>Bushing, Coupling, BI, Inside Thread, 1" Dia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brush, Coarse Wire Wheel, 1/4" Hex Shank, 1-1/2" </t>
+  </si>
+  <si>
     <t>Brush, Wheel, Crimped, 1/4" Hex Shank, 1"</t>
   </si>
   <si>
@@ -2790,12 +2796,6 @@
   </si>
   <si>
     <t>Brush, Wheel, Crimped, 1/4" Hex Shank, 3"</t>
-  </si>
-  <si>
-    <t>Bushing, Coupling, BI, Inside Thread, 1" Dia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brush, Coarse Wire Wheel, 1/4" Hex Shank, 1-1/2" </t>
   </si>
   <si>
     <t>CON-CON_1329</t>
@@ -26491,7 +26491,9 @@
       <c r="A439" s="1">
         <v>429</v>
       </c>
-      <c r="B439" s="1"/>
+      <c r="B439" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C439" s="1"/>
       <c r="D439" s="1"/>
       <c r="E439" s="1" t="s">
@@ -26506,30 +26508,26 @@
       <c r="J439" s="1"/>
       <c r="K439" s="1"/>
       <c r="L439" s="3">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M439" s="3"/>
       <c r="N439" s="3">
         <v>0</v>
       </c>
       <c r="O439" s="3"/>
-      <c r="P439" s="3"/>
+      <c r="P439" s="3">
+        <v>60</v>
+      </c>
       <c r="Q439" s="2"/>
       <c r="R439" s="1" t="s">
         <v>23</v>
       </c>
       <c r="S439" s="1"/>
-      <c r="T439" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="T439" s="1"/>
       <c r="U439" s="1"/>
-      <c r="V439" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="V439" s="1"/>
       <c r="W439" s="1"/>
-      <c r="X439" s="1" t="s">
-        <v>288</v>
-      </c>
+      <c r="X439" s="1"/>
       <c r="Y439" s="1"/>
       <c r="Z439" s="1"/>
     </row>
@@ -26556,7 +26554,7 @@
       </c>
       <c r="M440" s="3"/>
       <c r="N440" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O440" s="3"/>
       <c r="P440" s="3"/>
@@ -26629,9 +26627,7 @@
       <c r="A442" s="1">
         <v>432</v>
       </c>
-      <c r="B442" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B442" s="1"/>
       <c r="C442" s="1"/>
       <c r="D442" s="1"/>
       <c r="E442" s="1" t="s">
@@ -26646,26 +26642,30 @@
       <c r="J442" s="1"/>
       <c r="K442" s="1"/>
       <c r="L442" s="3">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M442" s="3"/>
       <c r="N442" s="3">
         <v>0</v>
       </c>
       <c r="O442" s="3"/>
-      <c r="P442" s="3">
-        <v>60</v>
-      </c>
+      <c r="P442" s="3"/>
       <c r="Q442" s="2"/>
       <c r="R442" s="1" t="s">
         <v>23</v>
       </c>
       <c r="S442" s="1"/>
-      <c r="T442" s="1"/>
+      <c r="T442" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="U442" s="1"/>
-      <c r="V442" s="1"/>
+      <c r="V442" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="W442" s="1"/>
-      <c r="X442" s="1"/>
+      <c r="X442" s="1" t="s">
+        <v>288</v>
+      </c>
       <c r="Y442" s="1"/>
       <c r="Z442" s="1"/>
     </row>
@@ -26692,7 +26692,7 @@
       </c>
       <c r="M443" s="3"/>
       <c r="N443" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O443" s="3"/>
       <c r="P443" s="3"/>

</xml_diff>